<commit_message>
Test Case about Placing a Call added
Test Case Procedure Description step by step about Placing a Call added.
</commit_message>
<xml_diff>
--- a/Documents/TestProcedure/exe_002 - Scheduled feature Test Case Procedures.xlsx
+++ b/Documents/TestProcedure/exe_002 - Scheduled feature Test Case Procedures.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
   <si>
     <t>1.1.</t>
   </si>
@@ -127,6 +127,39 @@
   </si>
   <si>
     <t>Three messages were created and scheduled to be sent. Upon the date and time, messages were sent and receiver got the three messages.</t>
+  </si>
+  <si>
+    <t>Sender starts three conversations. Then, selecting a contact from the conversation list, the sender has the option to place a call for this contact.</t>
+  </si>
+  <si>
+    <t>1.3.1</t>
+  </si>
+  <si>
+    <t>Sender start three conversations by creating and sending three messages to a three diferent contacts.</t>
+  </si>
+  <si>
+    <t>1.3.2</t>
+  </si>
+  <si>
+    <t>Sender check the conversation list to select a contact.</t>
+  </si>
+  <si>
+    <t>1.3.3</t>
+  </si>
+  <si>
+    <t>Sender places a call to the just selected contact.</t>
+  </si>
+  <si>
+    <t>1.3.4</t>
+  </si>
+  <si>
+    <t>Efectively a call is placed to the selected contact.</t>
+  </si>
+  <si>
+    <t>Once a sender has three conversations at the same time, the sender select a contact from the conversation list to place a call. A new call should be placed to the selected contact.</t>
+  </si>
+  <si>
+    <t>Three conversations are started. Sender select a contact and places it a call. Efectively a call is placed to the selected contact from the conversation list.</t>
   </si>
 </sst>
 </file>
@@ -217,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -256,18 +289,24 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -571,9 +610,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -597,10 +638,10 @@
       <c r="B3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="17"/>
+      <c r="D3" s="15"/>
       <c r="E3" s="6" t="s">
         <v>10</v>
       </c>
@@ -615,17 +656,17 @@
       <c r="A4" s="8">
         <v>1</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="16" t="s">
@@ -643,12 +684,12 @@
       <c r="F5" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="19" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="16"/>
       <c r="C6" s="9" t="s">
         <v>3</v>
@@ -658,10 +699,10 @@
       </c>
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
-      <c r="G6" s="13"/>
+      <c r="G6" s="19"/>
     </row>
     <row r="7" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="16"/>
       <c r="C7" s="9" t="s">
         <v>5</v>
@@ -671,10 +712,10 @@
       </c>
       <c r="E7" s="16"/>
       <c r="F7" s="16"/>
-      <c r="G7" s="13"/>
+      <c r="G7" s="19"/>
     </row>
     <row r="8" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="15"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="16"/>
       <c r="C8" s="9" t="s">
         <v>7</v>
@@ -684,10 +725,10 @@
       </c>
       <c r="E8" s="16"/>
       <c r="F8" s="16"/>
-      <c r="G8" s="13"/>
+      <c r="G8" s="19"/>
     </row>
     <row r="9" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="15"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="16"/>
       <c r="C9" s="9" t="s">
         <v>8</v>
@@ -697,10 +738,10 @@
       </c>
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
-      <c r="G9" s="13"/>
+      <c r="G9" s="19"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
+      <c r="A10" s="17"/>
       <c r="B10" s="16"/>
       <c r="C10" s="11"/>
       <c r="D10" s="12" t="s">
@@ -708,10 +749,10 @@
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
-      <c r="G10" s="13"/>
+      <c r="G10" s="19"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="16"/>
       <c r="C11" s="9" t="s">
         <v>9</v>
@@ -721,10 +762,10 @@
       </c>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
-      <c r="G11" s="13"/>
+      <c r="G11" s="19"/>
     </row>
     <row r="12" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="15">
+      <c r="A12" s="17">
         <v>1.2</v>
       </c>
       <c r="B12" s="16" t="s">
@@ -742,12 +783,12 @@
       <c r="F12" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="19" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="16"/>
       <c r="C13" s="11" t="s">
         <v>3</v>
@@ -757,10 +798,10 @@
       </c>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
-      <c r="G13" s="13"/>
+      <c r="G13" s="19"/>
     </row>
     <row r="14" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
+      <c r="A14" s="17"/>
       <c r="B14" s="16"/>
       <c r="C14" s="11" t="s">
         <v>5</v>
@@ -770,10 +811,10 @@
       </c>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
-      <c r="G14" s="13"/>
+      <c r="G14" s="19"/>
     </row>
     <row r="15" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="16"/>
       <c r="C15" s="11" t="s">
         <v>7</v>
@@ -783,10 +824,10 @@
       </c>
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
-      <c r="G15" s="13"/>
+      <c r="G15" s="19"/>
     </row>
     <row r="16" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="16"/>
       <c r="C16" s="11" t="s">
         <v>31</v>
@@ -796,10 +837,10 @@
       </c>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
-      <c r="G16" s="13"/>
+      <c r="G16" s="19"/>
     </row>
     <row r="17" spans="1:7" ht="51" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="16"/>
       <c r="C17" s="11" t="s">
         <v>32</v>
@@ -809,10 +850,77 @@
       </c>
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
-      <c r="G17" s="13"/>
+      <c r="G17" s="19"/>
+    </row>
+    <row r="18" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="17">
+        <v>1.3</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="G18" s="19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="17"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="19"/>
+    </row>
+    <row r="20" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="17"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="19"/>
+    </row>
+    <row r="21" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="17"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="17">
+    <mergeCell ref="G18:G21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="F18:F21"/>
+    <mergeCell ref="A18:A21"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="B5:B11"/>
     <mergeCell ref="A5:A11"/>

</xml_diff>

<commit_message>
Scheduled Messages Test Case Proc Description
Scheduled Messages Test Case Procedure Description, including the Test
Case Procedure to Place a Call to a contact from the Conversation List.
</commit_message>
<xml_diff>
--- a/Documents/TestProcedure/exe_002 - Scheduled feature Test Case Procedures.xlsx
+++ b/Documents/TestProcedure/exe_002 - Scheduled feature Test Case Procedures.xlsx
@@ -294,20 +294,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -612,9 +612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -638,10 +636,10 @@
       <c r="B3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="15"/>
+      <c r="D3" s="18"/>
       <c r="E3" s="6" t="s">
         <v>10</v>
       </c>
@@ -656,14 +654,14 @@
       <c r="A4" s="8">
         <v>1</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
@@ -684,7 +682,7 @@
       <c r="F5" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="15" t="s">
         <v>17</v>
       </c>
     </row>
@@ -699,7 +697,7 @@
       </c>
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
-      <c r="G6" s="19"/>
+      <c r="G6" s="15"/>
     </row>
     <row r="7" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="17"/>
@@ -712,7 +710,7 @@
       </c>
       <c r="E7" s="16"/>
       <c r="F7" s="16"/>
-      <c r="G7" s="19"/>
+      <c r="G7" s="15"/>
     </row>
     <row r="8" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="17"/>
@@ -725,7 +723,7 @@
       </c>
       <c r="E8" s="16"/>
       <c r="F8" s="16"/>
-      <c r="G8" s="19"/>
+      <c r="G8" s="15"/>
     </row>
     <row r="9" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
@@ -738,7 +736,7 @@
       </c>
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
-      <c r="G9" s="19"/>
+      <c r="G9" s="15"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
@@ -749,7 +747,7 @@
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
-      <c r="G10" s="19"/>
+      <c r="G10" s="15"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
@@ -762,7 +760,7 @@
       </c>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
-      <c r="G11" s="19"/>
+      <c r="G11" s="15"/>
     </row>
     <row r="12" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A12" s="17">
@@ -783,7 +781,7 @@
       <c r="F12" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="15" t="s">
         <v>17</v>
       </c>
     </row>
@@ -798,7 +796,7 @@
       </c>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
-      <c r="G13" s="19"/>
+      <c r="G13" s="15"/>
     </row>
     <row r="14" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
@@ -811,7 +809,7 @@
       </c>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
-      <c r="G14" s="19"/>
+      <c r="G14" s="15"/>
     </row>
     <row r="15" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A15" s="17"/>
@@ -824,7 +822,7 @@
       </c>
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
-      <c r="G15" s="19"/>
+      <c r="G15" s="15"/>
     </row>
     <row r="16" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
@@ -837,7 +835,7 @@
       </c>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
-      <c r="G16" s="19"/>
+      <c r="G16" s="15"/>
     </row>
     <row r="17" spans="1:7" ht="51" x14ac:dyDescent="0.25">
       <c r="A17" s="17"/>
@@ -850,7 +848,7 @@
       </c>
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
-      <c r="G17" s="19"/>
+      <c r="G17" s="15"/>
     </row>
     <row r="18" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A18" s="17">
@@ -871,7 +869,7 @@
       <c r="F18" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="G18" s="19" t="s">
+      <c r="G18" s="15" t="s">
         <v>17</v>
       </c>
     </row>
@@ -886,7 +884,7 @@
       </c>
       <c r="E19" s="16"/>
       <c r="F19" s="16"/>
-      <c r="G19" s="19"/>
+      <c r="G19" s="15"/>
     </row>
     <row r="20" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A20" s="17"/>
@@ -899,7 +897,7 @@
       </c>
       <c r="E20" s="16"/>
       <c r="F20" s="16"/>
-      <c r="G20" s="19"/>
+      <c r="G20" s="15"/>
     </row>
     <row r="21" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17"/>
@@ -912,15 +910,10 @@
       </c>
       <c r="E21" s="16"/>
       <c r="F21" s="16"/>
-      <c r="G21" s="19"/>
+      <c r="G21" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="G18:G21"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="E18:E21"/>
-    <mergeCell ref="F18:F21"/>
-    <mergeCell ref="A18:A21"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="B5:B11"/>
     <mergeCell ref="A5:A11"/>
@@ -933,6 +926,11 @@
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="G5:G11"/>
     <mergeCell ref="G12:G17"/>
+    <mergeCell ref="G18:G21"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="E18:E21"/>
+    <mergeCell ref="F18:F21"/>
+    <mergeCell ref="A18:A21"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>